<commit_message>
Added number of hypoP for each risk group
</commit_message>
<xml_diff>
--- a/Development/Results/functional.form.xlsx
+++ b/Development/Results/functional.form.xlsx
@@ -32,13 +32,13 @@
     <t xml:space="preserve">200.7</t>
   </si>
   <si>
-    <t xml:space="preserve">PTH24u + dCa24u</t>
+    <t xml:space="preserve">PTH24u + dCa</t>
   </si>
   <si>
     <t xml:space="preserve">211.1</t>
   </si>
   <si>
-    <t xml:space="preserve">PTH24u + dCorrCa24u</t>
+    <t xml:space="preserve">PTH24u + dCorrCa</t>
   </si>
   <si>
     <t xml:space="preserve">207.9</t>
@@ -56,13 +56,13 @@
     <t xml:space="preserve">182.7</t>
   </si>
   <si>
-    <t xml:space="preserve">dPTH + dCa24u</t>
+    <t xml:space="preserve">dPTH + dCa</t>
   </si>
   <si>
     <t xml:space="preserve">190.4</t>
   </si>
   <si>
-    <t xml:space="preserve">dPTH + dCorrCa24u</t>
+    <t xml:space="preserve">dPTH + dCorrCa</t>
   </si>
   <si>
     <t xml:space="preserve">188.3</t>

</xml_diff>